<commit_message>
Vector Formulation and Data upload
</commit_message>
<xml_diff>
--- a/Data/StorageCAPEX.xlsx
+++ b/Data/StorageCAPEX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee65a08843967445/Desktop/Master Ordner Konsti/03_Studium/Master/Sustainable Energy - Energy Systems Analysis/Masterarbeit/MasterThesis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C07896D1-B9AB-4068-9B8D-9D791C0809D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{C07896D1-B9AB-4068-9B8D-9D791C0809D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{122665AF-B236-41A6-9D85-8A245AA8D44E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{706CCCE1-668A-42AD-A820-FAE74361E941}"/>
+    <workbookView minimized="1" xWindow="2580" yWindow="2580" windowWidth="14400" windowHeight="7270" xr2:uid="{706CCCE1-668A-42AD-A820-FAE74361E941}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,13 +41,13 @@
     <t>Technology</t>
   </si>
   <si>
-    <t>CAPEX [EUR/kWh]</t>
-  </si>
-  <si>
     <t>BESS</t>
   </si>
   <si>
     <t>Pumped Hydro</t>
+  </si>
+  <si>
+    <t>CAPEX [EUR/kW]</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -435,12 +435,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>460</v>
@@ -448,7 +448,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>800</v>

</xml_diff>